<commit_message>
MTR192, MTR 193, MTR4903, MTR5332, MTR6082 updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UserOnboarding.xlsx
+++ b/src/test/resources/testdata/UserOnboarding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcemek\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B28DE0-A33A-458D-ABD0-6ACDED99F812}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F141F19E-86ED-4817-8564-22C8E1AEBF7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="4530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnderwritingMaintenance" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="238">
   <si>
     <t>URL</t>
   </si>
@@ -538,79 +538,187 @@
     <t>Whewlett</t>
   </si>
   <si>
-    <t>Casey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> McCorkle</t>
-  </si>
-  <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bryant </t>
-  </si>
-  <si>
-    <t>AGCMccorkle</t>
-  </si>
-  <si>
-    <t>AGJBryant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea </t>
-  </si>
-  <si>
-    <t>Zakiayyah</t>
-  </si>
-  <si>
-    <t>Young</t>
-  </si>
-  <si>
-    <t>Wesley</t>
-  </si>
-  <si>
-    <t>Wicklund</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>Parker</t>
-  </si>
-  <si>
-    <t>AGAHall</t>
-  </si>
-  <si>
-    <t>AGZYoung</t>
-  </si>
-  <si>
-    <t>AGWWicklund</t>
-  </si>
-  <si>
-    <t>AGJParker</t>
-  </si>
-  <si>
-    <t>Hall Maxwell</t>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Salgado</t>
+  </si>
+  <si>
+    <t>AGKBenson</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Benson</t>
+  </si>
+  <si>
+    <t>AGBMartinez</t>
+  </si>
+  <si>
+    <t>Brett</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>AGBGriffith</t>
+  </si>
+  <si>
+    <t>Brennan</t>
+  </si>
+  <si>
+    <t>Griffith</t>
+  </si>
+  <si>
+    <t>AGPMyers</t>
+  </si>
+  <si>
+    <t>Myers</t>
+  </si>
+  <si>
+    <t>AGJMcknight</t>
+  </si>
+  <si>
+    <t>Jabari</t>
+  </si>
+  <si>
+    <t>Mcknight</t>
+  </si>
+  <si>
+    <t>AGSFauceglia</t>
+  </si>
+  <si>
+    <t>Samantha</t>
+  </si>
+  <si>
+    <t>Fauceglia</t>
+  </si>
+  <si>
+    <t>AGTSalgado</t>
+  </si>
+  <si>
+    <t>Teyana</t>
+  </si>
+  <si>
+    <t>AGRJohnson</t>
+  </si>
+  <si>
+    <t>Ramina</t>
+  </si>
+  <si>
+    <t>AGFMurchison</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Murchison</t>
+  </si>
+  <si>
+    <t>AGCMintz</t>
+  </si>
+  <si>
+    <t>Mintz</t>
+  </si>
+  <si>
+    <t>AGASManns</t>
+  </si>
+  <si>
+    <t>Altrea</t>
+  </si>
+  <si>
+    <t>Manns</t>
+  </si>
+  <si>
+    <t>AGCHaines</t>
+  </si>
+  <si>
+    <t>Haines</t>
+  </si>
+  <si>
+    <t>AGFMWilliams</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>AGTEJann</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Jann</t>
+  </si>
+  <si>
+    <t>AGCLRamsey</t>
+  </si>
+  <si>
+    <t>Chanelle</t>
+  </si>
+  <si>
+    <t>Ramsey</t>
   </si>
   <si>
     <t>800-676-0769</t>
   </si>
   <si>
-    <t>casey.mccorkle@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>jason.bryant@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>andrea.hall-maxwell@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>kia.young@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>wesley.wicklund@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>jessica.parker@guidedsolutions.com</t>
+    <t>kevin.benson@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>brett.martinez@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>brennan.griffith@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>patrick.myers@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>jabari.mcknight@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>samantha.fauceglia@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>teyana.salgado@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>ramina.johnson@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>fred.murchison@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>christopher.mintz@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>altrea.manns@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>cole.haines@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>frances.williams@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>thomas.jann@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>chanelle.ramsey@guidedsolutions.com</t>
   </si>
   <si>
     <t>AG9400A1</t>
@@ -738,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -786,7 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1111,51 +1218,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FM116"/>
   <sheetViews>
-    <sheetView topLeftCell="DX1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="DP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="ED10" sqref="ED10"/>
+      <selection pane="bottomLeft" activeCell="EC1" sqref="EC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="13" width="12.109375" style="6"/>
-    <col min="14" max="14" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" style="6"/>
-    <col min="16" max="16" width="22.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" style="6"/>
+    <col min="1" max="13" width="12.1015625" style="6"/>
+    <col min="14" max="14" width="11.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1015625" style="6"/>
+    <col min="16" max="16" width="22.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1015625" style="6"/>
     <col min="18" max="18" width="25" style="6" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="24" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="38" width="12.109375" style="6"/>
-    <col min="39" max="39" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.33203125" style="6" customWidth="1"/>
-    <col min="42" max="42" width="14.109375" style="6" customWidth="1"/>
-    <col min="43" max="46" width="12.109375" style="6"/>
+    <col min="21" max="38" width="12.1015625" style="6"/>
+    <col min="39" max="39" width="16.3125" style="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.3125" style="6" customWidth="1"/>
+    <col min="42" max="42" width="14.1015625" style="6" customWidth="1"/>
+    <col min="43" max="46" width="12.1015625" style="6"/>
     <col min="47" max="47" width="24" style="6" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.44140625" style="6" customWidth="1"/>
-    <col min="49" max="80" width="12.109375" style="6"/>
-    <col min="81" max="81" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="82" max="155" width="12.109375" style="6"/>
-    <col min="156" max="156" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="30.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="12.109375" style="6"/>
-    <col min="159" max="159" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="30.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="12.109375" style="6"/>
-    <col min="162" max="162" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="30.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="12.109375" style="6"/>
-    <col min="165" max="165" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="30.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="12.109375" style="6"/>
-    <col min="168" max="168" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="30.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="170" max="16384" width="12.109375" style="6"/>
+    <col min="48" max="48" width="16.41796875" style="6" customWidth="1"/>
+    <col min="49" max="80" width="12.1015625" style="6"/>
+    <col min="81" max="81" width="21.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="82" max="155" width="12.1015625" style="6"/>
+    <col min="156" max="156" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="30.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="12.1015625" style="6"/>
+    <col min="159" max="159" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="30.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="12.1015625" style="6"/>
+    <col min="162" max="162" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="30.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="12.1015625" style="6"/>
+    <col min="165" max="165" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="30.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="12.1015625" style="6"/>
+    <col min="168" max="168" width="13.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="30.5234375" style="6" bestFit="1" customWidth="1"/>
+    <col min="170" max="16384" width="12.1015625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:169" s="22" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:169" s="22" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1552,8 +1659,8 @@
       <c r="EB1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="EC1" s="30" t="s">
-        <v>201</v>
+      <c r="EC1" s="29" t="s">
+        <v>237</v>
       </c>
       <c r="ED1" s="21" t="s">
         <v>63</v>
@@ -1664,11 +1771,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:169" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:169" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="22"/>
       <c r="E2" s="3"/>
       <c r="F2" s="23" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>130</v>
@@ -1761,8 +1868,8 @@
       <c r="AN2" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="AO2" s="29" t="s">
-        <v>199</v>
+      <c r="AO2" s="28" t="s">
+        <v>235</v>
       </c>
       <c r="AP2" s="9" t="s">
         <v>140</v>
@@ -1866,8 +1973,8 @@
       <c r="CB2" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="CC2" s="29" t="s">
-        <v>199</v>
+      <c r="CC2" s="28" t="s">
+        <v>235</v>
       </c>
       <c r="CD2" s="18" t="s">
         <v>146</v>
@@ -1990,17 +2097,17 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:169" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:169" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="22"/>
       <c r="E3" s="3"/>
       <c r="F3" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>131</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>161</v>
@@ -2089,8 +2196,8 @@
       <c r="AN3" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="AO3" s="29" t="s">
-        <v>200</v>
+      <c r="AO3" s="28" t="s">
+        <v>236</v>
       </c>
       <c r="AP3" s="9" t="s">
         <v>140</v>
@@ -2194,8 +2301,8 @@
       <c r="CB3" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="CC3" s="29" t="s">
-        <v>200</v>
+      <c r="CC3" s="28" t="s">
+        <v>236</v>
       </c>
       <c r="CD3" s="18" t="s">
         <v>146</v>
@@ -2408,7 +2515,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K4" s="7"/>
       <c r="N4" s="7"/>
       <c r="CI4" s="7"/>
@@ -2425,7 +2532,7 @@
       <c r="DX4" s="8"/>
       <c r="DY4" s="8"/>
     </row>
-    <row r="5" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K5" s="7"/>
       <c r="N5" s="7"/>
       <c r="CI5" s="7"/>
@@ -2442,7 +2549,7 @@
       <c r="DX5" s="8"/>
       <c r="DY5" s="8"/>
     </row>
-    <row r="6" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K6" s="7"/>
       <c r="N6" s="7"/>
       <c r="CI6" s="7"/>
@@ -2459,7 +2566,7 @@
       <c r="DX6" s="8"/>
       <c r="DY6" s="8"/>
     </row>
-    <row r="7" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K7" s="7"/>
       <c r="N7" s="7"/>
       <c r="CI7" s="7"/>
@@ -2476,7 +2583,7 @@
       <c r="DX7" s="8"/>
       <c r="DY7" s="8"/>
     </row>
-    <row r="8" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K8" s="7"/>
       <c r="N8" s="7"/>
       <c r="CH8" s="7"/>
@@ -2493,7 +2600,7 @@
       <c r="DW8" s="8"/>
       <c r="DX8" s="8"/>
     </row>
-    <row r="9" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K9" s="7"/>
       <c r="N9" s="7"/>
       <c r="CH9" s="7"/>
@@ -2510,7 +2617,7 @@
       <c r="DW9" s="8"/>
       <c r="DX9" s="8"/>
     </row>
-    <row r="10" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K10" s="7"/>
       <c r="N10" s="7"/>
       <c r="CH10" s="7"/>
@@ -2527,7 +2634,7 @@
       <c r="DW10" s="8"/>
       <c r="DX10" s="8"/>
     </row>
-    <row r="11" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K11" s="7"/>
       <c r="N11" s="7"/>
       <c r="CH11" s="7"/>
@@ -2544,7 +2651,7 @@
       <c r="DW11" s="8"/>
       <c r="DX11" s="8"/>
     </row>
-    <row r="12" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K12" s="7"/>
       <c r="N12" s="7"/>
       <c r="CH12" s="7"/>
@@ -2561,7 +2668,7 @@
       <c r="DW12" s="8"/>
       <c r="DX12" s="8"/>
     </row>
-    <row r="13" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K13" s="7"/>
       <c r="N13" s="7"/>
       <c r="CH13" s="7"/>
@@ -2578,7 +2685,7 @@
       <c r="DW13" s="8"/>
       <c r="DX13" s="8"/>
     </row>
-    <row r="14" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K14" s="7"/>
       <c r="N14" s="7"/>
       <c r="CH14" s="7"/>
@@ -2595,7 +2702,7 @@
       <c r="DW14" s="8"/>
       <c r="DX14" s="8"/>
     </row>
-    <row r="15" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K15" s="7"/>
       <c r="N15" s="7"/>
       <c r="CH15" s="7"/>
@@ -2612,7 +2719,7 @@
       <c r="DW15" s="8"/>
       <c r="DX15" s="8"/>
     </row>
-    <row r="16" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:169" x14ac:dyDescent="0.55000000000000004">
       <c r="K16" s="7"/>
       <c r="N16" s="7"/>
       <c r="CI16" s="7"/>
@@ -2629,7 +2736,7 @@
       <c r="DX16" s="8"/>
       <c r="DY16" s="8"/>
     </row>
-    <row r="17" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="17" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K17" s="7"/>
       <c r="N17" s="7"/>
       <c r="CI17" s="7"/>
@@ -2646,7 +2753,7 @@
       <c r="DX17" s="8"/>
       <c r="DY17" s="8"/>
     </row>
-    <row r="18" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K18" s="7"/>
       <c r="N18" s="7"/>
       <c r="CI18" s="7"/>
@@ -2663,7 +2770,7 @@
       <c r="DX18" s="8"/>
       <c r="DY18" s="8"/>
     </row>
-    <row r="19" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K19" s="7"/>
       <c r="N19" s="7"/>
       <c r="CI19" s="7"/>
@@ -2680,7 +2787,7 @@
       <c r="DX19" s="8"/>
       <c r="DY19" s="8"/>
     </row>
-    <row r="20" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K20" s="7"/>
       <c r="N20" s="7"/>
       <c r="CI20" s="7"/>
@@ -2697,7 +2804,7 @@
       <c r="DX20" s="8"/>
       <c r="DY20" s="8"/>
     </row>
-    <row r="21" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K21" s="7"/>
       <c r="N21" s="7"/>
       <c r="CI21" s="7"/>
@@ -2714,7 +2821,7 @@
       <c r="DX21" s="8"/>
       <c r="DY21" s="8"/>
     </row>
-    <row r="22" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="22" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K22" s="7"/>
       <c r="N22" s="7"/>
       <c r="CI22" s="7"/>
@@ -2731,7 +2838,7 @@
       <c r="DX22" s="8"/>
       <c r="DY22" s="8"/>
     </row>
-    <row r="23" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="23" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K23" s="7"/>
       <c r="N23" s="7"/>
       <c r="CI23" s="7"/>
@@ -2748,7 +2855,7 @@
       <c r="DX23" s="8"/>
       <c r="DY23" s="8"/>
     </row>
-    <row r="24" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K24" s="7"/>
       <c r="N24" s="7"/>
       <c r="CI24" s="7"/>
@@ -2765,7 +2872,7 @@
       <c r="DX24" s="8"/>
       <c r="DY24" s="8"/>
     </row>
-    <row r="25" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="25" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K25" s="7"/>
       <c r="N25" s="7"/>
       <c r="CI25" s="7"/>
@@ -2782,7 +2889,7 @@
       <c r="DX25" s="8"/>
       <c r="DY25" s="8"/>
     </row>
-    <row r="26" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="26" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K26" s="7"/>
       <c r="N26" s="7"/>
       <c r="CI26" s="7"/>
@@ -2799,7 +2906,7 @@
       <c r="DX26" s="8"/>
       <c r="DY26" s="8"/>
     </row>
-    <row r="27" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="27" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K27" s="7"/>
       <c r="N27" s="7"/>
       <c r="CI27" s="7"/>
@@ -2816,7 +2923,7 @@
       <c r="DX27" s="8"/>
       <c r="DY27" s="8"/>
     </row>
-    <row r="28" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="28" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K28" s="7"/>
       <c r="N28" s="7"/>
       <c r="CI28" s="7"/>
@@ -2833,7 +2940,7 @@
       <c r="DX28" s="8"/>
       <c r="DY28" s="8"/>
     </row>
-    <row r="29" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="29" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K29" s="7"/>
       <c r="N29" s="7"/>
       <c r="CI29" s="7"/>
@@ -2850,7 +2957,7 @@
       <c r="DX29" s="8"/>
       <c r="DY29" s="8"/>
     </row>
-    <row r="30" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="30" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K30" s="7"/>
       <c r="N30" s="7"/>
       <c r="CI30" s="7"/>
@@ -2867,7 +2974,7 @@
       <c r="DX30" s="8"/>
       <c r="DY30" s="8"/>
     </row>
-    <row r="31" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="31" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K31" s="7"/>
       <c r="N31" s="7"/>
       <c r="CI31" s="7"/>
@@ -2884,7 +2991,7 @@
       <c r="DX31" s="8"/>
       <c r="DY31" s="8"/>
     </row>
-    <row r="32" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="32" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K32" s="7"/>
       <c r="N32" s="7"/>
       <c r="CI32" s="7"/>
@@ -2901,7 +3008,7 @@
       <c r="DX32" s="8"/>
       <c r="DY32" s="8"/>
     </row>
-    <row r="33" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K33" s="7"/>
       <c r="N33" s="7"/>
       <c r="CI33" s="7"/>
@@ -2918,7 +3025,7 @@
       <c r="DX33" s="8"/>
       <c r="DY33" s="8"/>
     </row>
-    <row r="34" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K34" s="7"/>
       <c r="N34" s="7"/>
       <c r="CI34" s="7"/>
@@ -2935,7 +3042,7 @@
       <c r="DX34" s="8"/>
       <c r="DY34" s="8"/>
     </row>
-    <row r="35" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K35" s="7"/>
       <c r="N35" s="7"/>
       <c r="CI35" s="7"/>
@@ -2952,7 +3059,7 @@
       <c r="DX35" s="8"/>
       <c r="DY35" s="8"/>
     </row>
-    <row r="36" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K36" s="7"/>
       <c r="N36" s="7"/>
       <c r="CI36" s="7"/>
@@ -2969,7 +3076,7 @@
       <c r="DX36" s="8"/>
       <c r="DY36" s="8"/>
     </row>
-    <row r="37" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="37" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K37" s="7"/>
       <c r="N37" s="7"/>
       <c r="CI37" s="7"/>
@@ -2986,7 +3093,7 @@
       <c r="DX37" s="8"/>
       <c r="DY37" s="8"/>
     </row>
-    <row r="38" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="38" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K38" s="7"/>
       <c r="N38" s="7"/>
       <c r="CI38" s="7"/>
@@ -3003,7 +3110,7 @@
       <c r="DX38" s="8"/>
       <c r="DY38" s="8"/>
     </row>
-    <row r="39" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="39" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K39" s="7"/>
       <c r="N39" s="7"/>
       <c r="CI39" s="7"/>
@@ -3020,7 +3127,7 @@
       <c r="DX39" s="8"/>
       <c r="DY39" s="8"/>
     </row>
-    <row r="40" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="40" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K40" s="7"/>
       <c r="N40" s="7"/>
       <c r="CI40" s="7"/>
@@ -3037,7 +3144,7 @@
       <c r="DX40" s="8"/>
       <c r="DY40" s="8"/>
     </row>
-    <row r="41" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="41" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K41" s="7"/>
       <c r="N41" s="7"/>
       <c r="CI41" s="7"/>
@@ -3054,7 +3161,7 @@
       <c r="DX41" s="8"/>
       <c r="DY41" s="8"/>
     </row>
-    <row r="42" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="42" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K42" s="7"/>
       <c r="N42" s="7"/>
       <c r="CI42" s="7"/>
@@ -3071,7 +3178,7 @@
       <c r="DX42" s="8"/>
       <c r="DY42" s="8"/>
     </row>
-    <row r="43" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="43" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K43" s="7"/>
       <c r="N43" s="7"/>
       <c r="CI43" s="7"/>
@@ -3088,7 +3195,7 @@
       <c r="DX43" s="8"/>
       <c r="DY43" s="8"/>
     </row>
-    <row r="44" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="44" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K44" s="7"/>
       <c r="N44" s="7"/>
       <c r="CI44" s="7"/>
@@ -3105,7 +3212,7 @@
       <c r="DX44" s="8"/>
       <c r="DY44" s="8"/>
     </row>
-    <row r="45" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="45" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K45" s="7"/>
       <c r="N45" s="7"/>
       <c r="CI45" s="7"/>
@@ -3122,7 +3229,7 @@
       <c r="DX45" s="8"/>
       <c r="DY45" s="8"/>
     </row>
-    <row r="46" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="46" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K46" s="7"/>
       <c r="N46" s="7"/>
       <c r="CI46" s="7"/>
@@ -3139,7 +3246,7 @@
       <c r="DX46" s="8"/>
       <c r="DY46" s="8"/>
     </row>
-    <row r="47" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="47" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K47" s="7"/>
       <c r="N47" s="7"/>
       <c r="CI47" s="7"/>
@@ -3156,7 +3263,7 @@
       <c r="DX47" s="8"/>
       <c r="DY47" s="8"/>
     </row>
-    <row r="48" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="48" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K48" s="7"/>
       <c r="N48" s="7"/>
       <c r="CI48" s="7"/>
@@ -3173,7 +3280,7 @@
       <c r="DX48" s="8"/>
       <c r="DY48" s="8"/>
     </row>
-    <row r="49" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="49" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K49" s="7"/>
       <c r="N49" s="7"/>
       <c r="CI49" s="7"/>
@@ -3190,7 +3297,7 @@
       <c r="DX49" s="8"/>
       <c r="DY49" s="8"/>
     </row>
-    <row r="50" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="50" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K50" s="7"/>
       <c r="N50" s="7"/>
       <c r="CI50" s="7"/>
@@ -3207,7 +3314,7 @@
       <c r="DX50" s="8"/>
       <c r="DY50" s="8"/>
     </row>
-    <row r="51" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="51" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K51" s="7"/>
       <c r="N51" s="7"/>
       <c r="CI51" s="7"/>
@@ -3224,7 +3331,7 @@
       <c r="DX51" s="8"/>
       <c r="DY51" s="8"/>
     </row>
-    <row r="52" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="52" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K52" s="7"/>
       <c r="N52" s="7"/>
       <c r="CI52" s="7"/>
@@ -3241,7 +3348,7 @@
       <c r="DX52" s="8"/>
       <c r="DY52" s="8"/>
     </row>
-    <row r="53" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="53" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K53" s="7"/>
       <c r="N53" s="7"/>
       <c r="CI53" s="7"/>
@@ -3258,7 +3365,7 @@
       <c r="DX53" s="8"/>
       <c r="DY53" s="8"/>
     </row>
-    <row r="54" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="54" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K54" s="7"/>
       <c r="N54" s="7"/>
       <c r="CI54" s="7"/>
@@ -3275,7 +3382,7 @@
       <c r="DX54" s="8"/>
       <c r="DY54" s="8"/>
     </row>
-    <row r="55" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="55" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K55" s="7"/>
       <c r="N55" s="7"/>
       <c r="CI55" s="7"/>
@@ -3292,7 +3399,7 @@
       <c r="DX55" s="8"/>
       <c r="DY55" s="8"/>
     </row>
-    <row r="56" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="56" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K56" s="7"/>
       <c r="N56" s="7"/>
       <c r="CI56" s="7"/>
@@ -3309,7 +3416,7 @@
       <c r="DX56" s="8"/>
       <c r="DY56" s="8"/>
     </row>
-    <row r="57" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="57" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K57" s="7"/>
       <c r="N57" s="7"/>
       <c r="CI57" s="7"/>
@@ -3326,7 +3433,7 @@
       <c r="DX57" s="8"/>
       <c r="DY57" s="8"/>
     </row>
-    <row r="58" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="58" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K58" s="7"/>
       <c r="N58" s="7"/>
       <c r="CI58" s="7"/>
@@ -3343,7 +3450,7 @@
       <c r="DX58" s="8"/>
       <c r="DY58" s="8"/>
     </row>
-    <row r="59" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="59" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K59" s="7"/>
       <c r="N59" s="7"/>
       <c r="CI59" s="7"/>
@@ -3360,7 +3467,7 @@
       <c r="DX59" s="8"/>
       <c r="DY59" s="8"/>
     </row>
-    <row r="60" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="60" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K60" s="7"/>
       <c r="N60" s="7"/>
       <c r="CI60" s="7"/>
@@ -3377,7 +3484,7 @@
       <c r="DX60" s="8"/>
       <c r="DY60" s="8"/>
     </row>
-    <row r="61" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="61" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K61" s="7"/>
       <c r="N61" s="7"/>
       <c r="CI61" s="7"/>
@@ -3394,7 +3501,7 @@
       <c r="DX61" s="8"/>
       <c r="DY61" s="8"/>
     </row>
-    <row r="62" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="62" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K62" s="7"/>
       <c r="N62" s="7"/>
       <c r="CI62" s="7"/>
@@ -3411,7 +3518,7 @@
       <c r="DX62" s="8"/>
       <c r="DY62" s="8"/>
     </row>
-    <row r="63" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="63" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K63" s="7"/>
       <c r="N63" s="7"/>
       <c r="CI63" s="7"/>
@@ -3428,7 +3535,7 @@
       <c r="DX63" s="8"/>
       <c r="DY63" s="8"/>
     </row>
-    <row r="64" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="64" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K64" s="7"/>
       <c r="N64" s="7"/>
       <c r="CI64" s="7"/>
@@ -3445,7 +3552,7 @@
       <c r="DX64" s="8"/>
       <c r="DY64" s="8"/>
     </row>
-    <row r="65" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="65" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K65" s="7"/>
       <c r="N65" s="7"/>
       <c r="CI65" s="7"/>
@@ -3462,7 +3569,7 @@
       <c r="DX65" s="8"/>
       <c r="DY65" s="8"/>
     </row>
-    <row r="66" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="66" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K66" s="7"/>
       <c r="N66" s="7"/>
       <c r="CI66" s="7"/>
@@ -3479,7 +3586,7 @@
       <c r="DX66" s="8"/>
       <c r="DY66" s="8"/>
     </row>
-    <row r="67" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="67" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K67" s="7"/>
       <c r="N67" s="7"/>
       <c r="CI67" s="7"/>
@@ -3496,7 +3603,7 @@
       <c r="DX67" s="8"/>
       <c r="DY67" s="8"/>
     </row>
-    <row r="68" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="68" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K68" s="7"/>
       <c r="N68" s="7"/>
       <c r="CI68" s="7"/>
@@ -3513,7 +3620,7 @@
       <c r="DX68" s="8"/>
       <c r="DY68" s="8"/>
     </row>
-    <row r="69" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="69" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K69" s="7"/>
       <c r="N69" s="7"/>
       <c r="CI69" s="7"/>
@@ -3530,7 +3637,7 @@
       <c r="DX69" s="8"/>
       <c r="DY69" s="8"/>
     </row>
-    <row r="70" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="70" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K70" s="7"/>
       <c r="N70" s="7"/>
       <c r="CI70" s="7"/>
@@ -3547,7 +3654,7 @@
       <c r="DX70" s="8"/>
       <c r="DY70" s="8"/>
     </row>
-    <row r="71" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="71" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K71" s="7"/>
       <c r="N71" s="7"/>
       <c r="CI71" s="7"/>
@@ -3564,7 +3671,7 @@
       <c r="DX71" s="8"/>
       <c r="DY71" s="8"/>
     </row>
-    <row r="72" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="72" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K72" s="7"/>
       <c r="N72" s="7"/>
       <c r="CI72" s="7"/>
@@ -3581,7 +3688,7 @@
       <c r="DX72" s="8"/>
       <c r="DY72" s="8"/>
     </row>
-    <row r="73" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="73" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K73" s="7"/>
       <c r="N73" s="7"/>
       <c r="CI73" s="7"/>
@@ -3598,7 +3705,7 @@
       <c r="DX73" s="8"/>
       <c r="DY73" s="8"/>
     </row>
-    <row r="74" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="74" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K74" s="7"/>
       <c r="N74" s="7"/>
       <c r="CI74" s="7"/>
@@ -3615,7 +3722,7 @@
       <c r="DX74" s="8"/>
       <c r="DY74" s="8"/>
     </row>
-    <row r="75" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="75" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K75" s="7"/>
       <c r="N75" s="7"/>
       <c r="CI75" s="7"/>
@@ -3632,7 +3739,7 @@
       <c r="DX75" s="8"/>
       <c r="DY75" s="8"/>
     </row>
-    <row r="76" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="76" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K76" s="7"/>
       <c r="N76" s="7"/>
       <c r="CI76" s="7"/>
@@ -3649,7 +3756,7 @@
       <c r="DX76" s="8"/>
       <c r="DY76" s="8"/>
     </row>
-    <row r="77" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="77" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K77" s="7"/>
       <c r="N77" s="7"/>
       <c r="CI77" s="7"/>
@@ -3666,7 +3773,7 @@
       <c r="DX77" s="8"/>
       <c r="DY77" s="8"/>
     </row>
-    <row r="78" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="78" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K78" s="7"/>
       <c r="N78" s="7"/>
       <c r="CI78" s="7"/>
@@ -3683,7 +3790,7 @@
       <c r="DX78" s="8"/>
       <c r="DY78" s="8"/>
     </row>
-    <row r="79" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="79" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K79" s="7"/>
       <c r="N79" s="7"/>
       <c r="CI79" s="7"/>
@@ -3700,7 +3807,7 @@
       <c r="DX79" s="8"/>
       <c r="DY79" s="8"/>
     </row>
-    <row r="80" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="80" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K80" s="7"/>
       <c r="N80" s="7"/>
       <c r="CI80" s="7"/>
@@ -3717,7 +3824,7 @@
       <c r="DX80" s="8"/>
       <c r="DY80" s="8"/>
     </row>
-    <row r="81" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="81" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K81" s="7"/>
       <c r="N81" s="7"/>
       <c r="CI81" s="7"/>
@@ -3734,7 +3841,7 @@
       <c r="DX81" s="8"/>
       <c r="DY81" s="8"/>
     </row>
-    <row r="82" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="82" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K82" s="7"/>
       <c r="N82" s="7"/>
       <c r="CI82" s="7"/>
@@ -3751,7 +3858,7 @@
       <c r="DX82" s="8"/>
       <c r="DY82" s="8"/>
     </row>
-    <row r="83" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="83" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K83" s="7"/>
       <c r="N83" s="7"/>
       <c r="CI83" s="7"/>
@@ -3768,7 +3875,7 @@
       <c r="DX83" s="8"/>
       <c r="DY83" s="8"/>
     </row>
-    <row r="84" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="84" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K84" s="7"/>
       <c r="N84" s="7"/>
       <c r="CI84" s="7"/>
@@ -3785,7 +3892,7 @@
       <c r="DX84" s="8"/>
       <c r="DY84" s="8"/>
     </row>
-    <row r="85" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="85" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K85" s="7"/>
       <c r="N85" s="7"/>
       <c r="CI85" s="7"/>
@@ -3802,7 +3909,7 @@
       <c r="DX85" s="8"/>
       <c r="DY85" s="8"/>
     </row>
-    <row r="86" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="86" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K86" s="7"/>
       <c r="N86" s="7"/>
       <c r="CI86" s="7"/>
@@ -3819,7 +3926,7 @@
       <c r="DX86" s="8"/>
       <c r="DY86" s="8"/>
     </row>
-    <row r="87" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="87" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K87" s="7"/>
       <c r="N87" s="7"/>
       <c r="CI87" s="7"/>
@@ -3836,7 +3943,7 @@
       <c r="DX87" s="8"/>
       <c r="DY87" s="8"/>
     </row>
-    <row r="88" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="88" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K88" s="7"/>
       <c r="N88" s="7"/>
       <c r="CI88" s="7"/>
@@ -3853,7 +3960,7 @@
       <c r="DX88" s="8"/>
       <c r="DY88" s="8"/>
     </row>
-    <row r="89" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="89" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K89" s="7"/>
       <c r="N89" s="7"/>
       <c r="CI89" s="7"/>
@@ -3870,7 +3977,7 @@
       <c r="DX89" s="8"/>
       <c r="DY89" s="8"/>
     </row>
-    <row r="90" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="90" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K90" s="7"/>
       <c r="N90" s="7"/>
       <c r="CI90" s="7"/>
@@ -3887,7 +3994,7 @@
       <c r="DX90" s="8"/>
       <c r="DY90" s="8"/>
     </row>
-    <row r="91" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="91" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K91" s="7"/>
       <c r="N91" s="7"/>
       <c r="CI91" s="7"/>
@@ -3904,7 +4011,7 @@
       <c r="DX91" s="8"/>
       <c r="DY91" s="8"/>
     </row>
-    <row r="92" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="92" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K92" s="7"/>
       <c r="N92" s="7"/>
       <c r="CI92" s="7"/>
@@ -3921,7 +4028,7 @@
       <c r="DX92" s="8"/>
       <c r="DY92" s="8"/>
     </row>
-    <row r="93" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="93" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K93" s="7"/>
       <c r="N93" s="7"/>
       <c r="CI93" s="7"/>
@@ -3938,7 +4045,7 @@
       <c r="DX93" s="8"/>
       <c r="DY93" s="8"/>
     </row>
-    <row r="94" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="94" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K94" s="7"/>
       <c r="N94" s="7"/>
       <c r="CI94" s="7"/>
@@ -3955,7 +4062,7 @@
       <c r="DX94" s="8"/>
       <c r="DY94" s="8"/>
     </row>
-    <row r="95" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="95" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K95" s="7"/>
       <c r="N95" s="7"/>
       <c r="CI95" s="7"/>
@@ -3972,7 +4079,7 @@
       <c r="DX95" s="8"/>
       <c r="DY95" s="8"/>
     </row>
-    <row r="96" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="96" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K96" s="7"/>
       <c r="N96" s="7"/>
       <c r="CI96" s="7"/>
@@ -3989,7 +4096,7 @@
       <c r="DX96" s="8"/>
       <c r="DY96" s="8"/>
     </row>
-    <row r="97" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="97" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K97" s="7"/>
       <c r="N97" s="7"/>
       <c r="CI97" s="7"/>
@@ -4006,7 +4113,7 @@
       <c r="DX97" s="8"/>
       <c r="DY97" s="8"/>
     </row>
-    <row r="98" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="98" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K98" s="7"/>
       <c r="N98" s="7"/>
       <c r="CI98" s="7"/>
@@ -4023,7 +4130,7 @@
       <c r="DX98" s="8"/>
       <c r="DY98" s="8"/>
     </row>
-    <row r="99" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="99" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K99" s="7"/>
       <c r="N99" s="7"/>
       <c r="CI99" s="7"/>
@@ -4040,7 +4147,7 @@
       <c r="DX99" s="8"/>
       <c r="DY99" s="8"/>
     </row>
-    <row r="100" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="100" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K100" s="7"/>
       <c r="N100" s="7"/>
       <c r="CI100" s="7"/>
@@ -4057,7 +4164,7 @@
       <c r="DX100" s="8"/>
       <c r="DY100" s="8"/>
     </row>
-    <row r="101" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="101" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K101" s="7"/>
       <c r="N101" s="7"/>
       <c r="CI101" s="7"/>
@@ -4074,7 +4181,7 @@
       <c r="DX101" s="8"/>
       <c r="DY101" s="8"/>
     </row>
-    <row r="102" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="102" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K102" s="7"/>
       <c r="N102" s="7"/>
       <c r="CI102" s="7"/>
@@ -4091,7 +4198,7 @@
       <c r="DX102" s="8"/>
       <c r="DY102" s="8"/>
     </row>
-    <row r="103" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="103" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K103" s="7"/>
       <c r="N103" s="7"/>
       <c r="CI103" s="7"/>
@@ -4108,7 +4215,7 @@
       <c r="DX103" s="8"/>
       <c r="DY103" s="8"/>
     </row>
-    <row r="104" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="104" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K104" s="7"/>
       <c r="N104" s="7"/>
       <c r="CI104" s="7"/>
@@ -4125,7 +4232,7 @@
       <c r="DX104" s="8"/>
       <c r="DY104" s="8"/>
     </row>
-    <row r="105" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="105" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K105" s="7"/>
       <c r="N105" s="7"/>
       <c r="CI105" s="7"/>
@@ -4142,7 +4249,7 @@
       <c r="DX105" s="8"/>
       <c r="DY105" s="8"/>
     </row>
-    <row r="106" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="106" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K106" s="7"/>
       <c r="N106" s="7"/>
       <c r="CI106" s="7"/>
@@ -4159,7 +4266,7 @@
       <c r="DX106" s="8"/>
       <c r="DY106" s="8"/>
     </row>
-    <row r="107" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="107" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K107" s="7"/>
       <c r="N107" s="7"/>
       <c r="CI107" s="7"/>
@@ -4176,7 +4283,7 @@
       <c r="DX107" s="8"/>
       <c r="DY107" s="8"/>
     </row>
-    <row r="108" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="108" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K108" s="7"/>
       <c r="N108" s="7"/>
       <c r="CI108" s="7"/>
@@ -4193,7 +4300,7 @@
       <c r="DX108" s="8"/>
       <c r="DY108" s="8"/>
     </row>
-    <row r="109" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="109" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K109" s="7"/>
       <c r="N109" s="7"/>
       <c r="CI109" s="7"/>
@@ -4210,7 +4317,7 @@
       <c r="DX109" s="8"/>
       <c r="DY109" s="8"/>
     </row>
-    <row r="110" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="110" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K110" s="7"/>
       <c r="N110" s="7"/>
       <c r="CI110" s="7"/>
@@ -4227,7 +4334,7 @@
       <c r="DX110" s="8"/>
       <c r="DY110" s="8"/>
     </row>
-    <row r="111" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="111" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K111" s="7"/>
       <c r="N111" s="7"/>
       <c r="CI111" s="7"/>
@@ -4244,7 +4351,7 @@
       <c r="DX111" s="8"/>
       <c r="DY111" s="8"/>
     </row>
-    <row r="112" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="112" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K112" s="7"/>
       <c r="N112" s="7"/>
       <c r="CI112" s="7"/>
@@ -4261,7 +4368,7 @@
       <c r="DX112" s="8"/>
       <c r="DY112" s="8"/>
     </row>
-    <row r="113" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="113" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K113" s="7"/>
       <c r="N113" s="7"/>
       <c r="CI113" s="7"/>
@@ -4278,7 +4385,7 @@
       <c r="DX113" s="8"/>
       <c r="DY113" s="8"/>
     </row>
-    <row r="114" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="114" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K114" s="7"/>
       <c r="N114" s="7"/>
       <c r="CI114" s="7"/>
@@ -4295,7 +4402,7 @@
       <c r="DX114" s="8"/>
       <c r="DY114" s="8"/>
     </row>
-    <row r="115" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="115" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K115" s="7"/>
       <c r="N115" s="7"/>
       <c r="CI115" s="7"/>
@@ -4312,7 +4419,7 @@
       <c r="DX115" s="8"/>
       <c r="DY115" s="8"/>
     </row>
-    <row r="116" spans="11:129" x14ac:dyDescent="0.3">
+    <row r="116" spans="11:129" x14ac:dyDescent="0.55000000000000004">
       <c r="K116" s="7"/>
       <c r="N116" s="7"/>
       <c r="CI116" s="7"/>
@@ -4343,63 +4450,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AM7"/>
+  <dimension ref="A1:AM16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="6"/>
-    <col min="10" max="10" width="19.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.68359375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.41796875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.89453125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="11.3125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.68359375" style="6"/>
+    <col min="10" max="10" width="19.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.89453125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.89453125" style="6" customWidth="1"/>
     <col min="13" max="13" width="15" style="6" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" style="6" customWidth="1"/>
-    <col min="15" max="16" width="8.6640625" style="6"/>
-    <col min="17" max="17" width="8.6640625" style="26"/>
-    <col min="18" max="18" width="8.6640625" style="6"/>
-    <col min="19" max="19" width="18.33203125" style="6" customWidth="1"/>
-    <col min="20" max="20" width="12.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="6" customWidth="1"/>
-    <col min="22" max="22" width="42.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5546875" style="6" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="15.5234375" style="6" customWidth="1"/>
+    <col min="15" max="16" width="8.68359375" style="6"/>
+    <col min="17" max="17" width="8.68359375" style="26"/>
+    <col min="18" max="18" width="8.68359375" style="6"/>
+    <col min="19" max="19" width="18.3125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="12.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.3125" style="6" customWidth="1"/>
+    <col min="22" max="22" width="42.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5234375" style="6" customWidth="1"/>
+    <col min="24" max="24" width="16.3125" style="6" customWidth="1"/>
     <col min="25" max="25" width="19" style="6" customWidth="1"/>
     <col min="26" max="26" width="29" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.6640625" style="6" customWidth="1"/>
-    <col min="28" max="28" width="25.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.68359375" style="6" customWidth="1"/>
+    <col min="28" max="28" width="25.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.1015625" style="6" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="29" style="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.6640625" style="6"/>
-    <col min="32" max="32" width="27.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.68359375" style="6"/>
+    <col min="32" max="32" width="27.89453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.3125" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.68359375" style="6" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="19" style="6" customWidth="1"/>
     <col min="36" max="36" width="21" style="6" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.6640625" style="6"/>
+    <col min="37" max="37" width="12.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.3125" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.68359375" style="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="8.68359375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:39" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -4511,10 +4618,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="27"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>121</v>
@@ -4529,10 +4635,10 @@
         <v>156</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>165</v>
@@ -4556,29 +4662,28 @@
         <v>138</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U2" s="6"/>
+        <v>215</v>
+      </c>
       <c r="V2" s="23" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="W2" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="Z2" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AC2" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="AD2" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AF2" s="19" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="AG2" s="20">
         <v>45394</v>
@@ -4596,10 +4701,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="3" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="27"/>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" s="23" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>121</v>
@@ -4614,10 +4718,10 @@
         <v>156</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="M3" s="23" t="s">
         <v>165</v>
@@ -4641,29 +4745,28 @@
         <v>138</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U3" s="6"/>
+        <v>215</v>
+      </c>
       <c r="V3" s="23" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="W3" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y3" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AC3" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="AD3" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AF3" s="19" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="AG3" s="20">
         <v>45394</v>
@@ -4681,10 +4784,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="4" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="27"/>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>121</v>
@@ -4699,10 +4801,10 @@
         <v>156</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>165</v>
@@ -4726,29 +4828,28 @@
         <v>138</v>
       </c>
       <c r="T4" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U4" s="6"/>
+        <v>215</v>
+      </c>
       <c r="V4" s="23" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="W4" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y4" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AC4" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AF4" s="19" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="AG4" s="20">
         <v>45394</v>
@@ -4766,10 +4867,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="5" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="27"/>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="F5" s="23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>121</v>
@@ -4784,10 +4884,10 @@
         <v>156</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="M5" s="23" t="s">
         <v>165</v>
@@ -4811,29 +4911,28 @@
         <v>138</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U5" s="6"/>
+        <v>215</v>
+      </c>
       <c r="V5" s="23" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="W5" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y5" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="Z5" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AC5" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="AD5" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AF5" s="19" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="AG5" s="20">
         <v>45394</v>
@@ -4851,10 +4950,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="6" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="27"/>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="F6" s="23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>121</v>
@@ -4869,10 +4967,10 @@
         <v>156</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="M6" s="23" t="s">
         <v>165</v>
@@ -4896,29 +4994,28 @@
         <v>138</v>
       </c>
       <c r="T6" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U6" s="6"/>
+        <v>215</v>
+      </c>
       <c r="V6" s="23" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="W6" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y6" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="Z6" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AC6" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="AD6" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AF6" s="19" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="AG6" s="20">
         <v>45394</v>
@@ -4936,10 +5033,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="7" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="27"/>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="F7" s="23" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>121</v>
@@ -4954,10 +5050,10 @@
         <v>156</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="M7" s="23" t="s">
         <v>165</v>
@@ -4981,29 +5077,28 @@
         <v>138</v>
       </c>
       <c r="T7" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U7" s="6"/>
+        <v>215</v>
+      </c>
       <c r="V7" s="23" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="W7" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y7" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="Z7" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AC7" s="23" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="AD7" s="23" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="AF7" s="19" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="AG7" s="20">
         <v>45394</v>
@@ -5018,6 +5113,753 @@
         <v>45394</v>
       </c>
       <c r="AM7" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="19">
+        <v>10</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S8" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V8" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="W8" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y8" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z8" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC8" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD8" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF8" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG8" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH8" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK8" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL8" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM8" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="19">
+        <v>10</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R9" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T9" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V9" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="W9" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y9" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z9" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC9" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD9" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF9" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG9" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH9" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK9" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL9" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM9" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="19">
+        <v>10</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T10" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V10" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="W10" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y10" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z10" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC10" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD10" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG10" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH10" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK10" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL10" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM10" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="19">
+        <v>10</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R11" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V11" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="W11" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y11" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z11" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC11" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD11" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF11" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG11" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH11" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK11" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL11" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM11" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="19">
+        <v>10</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P12" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S12" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T12" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V12" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="W12" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y12" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z12" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC12" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD12" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF12" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG12" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH12" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK12" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL12" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM12" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="19">
+        <v>10</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="M13" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T13" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V13" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="W13" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y13" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z13" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC13" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD13" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF13" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG13" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH13" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK13" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL13" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM13" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="19">
+        <v>10</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q14" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T14" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V14" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="W14" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y14" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z14" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC14" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD14" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF14" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG14" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH14" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK14" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL14" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM14" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" s="19">
+        <v>10</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T15" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V15" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="W15" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y15" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z15" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC15" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD15" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF15" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG15" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH15" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK15" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL15" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM15" s="20">
+        <v>2958465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="19">
+        <v>10</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P16" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q16" s="23">
+        <v>33634</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="T16" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="V16" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="W16" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y16" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z16" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC16" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD16" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="AF16" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG16" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AH16" s="20">
+        <v>2958465</v>
+      </c>
+      <c r="AK16" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL16" s="20">
+        <v>45394</v>
+      </c>
+      <c r="AM16" s="20">
         <v>2958465</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MTR-5523 MTR-194 MTR-191 MTR-190 MTR-347 MTR-344 MTR-346 MTR-342 MTR-341 MTR-343 VOLHO5 policy added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UserOnboarding.xlsx
+++ b/src/test/resources/testdata/UserOnboarding.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYavas\git\AutomationCucumber2023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B28DE0-A33A-458D-ABD0-6ACDED99F812}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E517EB-30BD-455F-A3A0-44A143D7B931}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="198">
   <si>
     <t>URL</t>
   </si>
@@ -538,79 +538,64 @@
     <t>Whewlett</t>
   </si>
   <si>
-    <t>Casey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> McCorkle</t>
-  </si>
-  <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bryant </t>
-  </si>
-  <si>
-    <t>AGCMccorkle</t>
-  </si>
-  <si>
-    <t>AGJBryant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea </t>
-  </si>
-  <si>
-    <t>Zakiayyah</t>
-  </si>
-  <si>
-    <t>Young</t>
-  </si>
-  <si>
-    <t>Wesley</t>
-  </si>
-  <si>
-    <t>Wicklund</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>Parker</t>
-  </si>
-  <si>
-    <t>AGAHall</t>
-  </si>
-  <si>
-    <t>AGZYoung</t>
-  </si>
-  <si>
-    <t>AGWWicklund</t>
-  </si>
-  <si>
-    <t>AGJParker</t>
-  </si>
-  <si>
-    <t>Hall Maxwell</t>
+    <t>AGJDSmith</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>AGCTye</t>
+  </si>
+  <si>
+    <t>Corey</t>
+  </si>
+  <si>
+    <t>Tye</t>
+  </si>
+  <si>
+    <t>AGKKeator</t>
+  </si>
+  <si>
+    <t>Kendall</t>
+  </si>
+  <si>
+    <t>Keator</t>
+  </si>
+  <si>
+    <t>AGTTownsend</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Townsend</t>
+  </si>
+  <si>
+    <t>AGGNelich</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Nelich</t>
   </si>
   <si>
     <t>800-676-0769</t>
   </si>
   <si>
-    <t>casey.mccorkle@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>jason.bryant@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>andrea.hall-maxwell@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>kia.young@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>wesley.wicklund@guidedsolutions.com</t>
-  </si>
-  <si>
-    <t>jessica.parker@guidedsolutions.com</t>
+    <t>joshua.smith@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>corey.tye@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>kendall.keator@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>tim.townsend@guidedsolutions.com</t>
+  </si>
+  <si>
+    <t>gabriel.nelich@guidedsolutions.com</t>
   </si>
   <si>
     <t>AG9400A1</t>
@@ -632,6 +617,9 @@
   </si>
   <si>
     <t>Line 5</t>
+  </si>
+  <si>
+    <t>Smithx</t>
   </si>
 </sst>
 </file>
@@ -738,7 +726,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -786,7 +774,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1111,10 +1098,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FM116"/>
   <sheetViews>
-    <sheetView topLeftCell="DX1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="DP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="ED10" sqref="ED10"/>
+      <selection pane="bottomLeft" activeCell="EC1" sqref="EC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,8 +1539,8 @@
       <c r="EB1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="EC1" s="30" t="s">
-        <v>201</v>
+      <c r="EC1" s="29" t="s">
+        <v>196</v>
       </c>
       <c r="ED1" s="21" t="s">
         <v>63</v>
@@ -1668,7 +1655,7 @@
       <c r="A2" s="22"/>
       <c r="E2" s="3"/>
       <c r="F2" s="23" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>130</v>
@@ -1761,8 +1748,8 @@
       <c r="AN2" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="AO2" s="29" t="s">
-        <v>199</v>
+      <c r="AO2" s="28" t="s">
+        <v>194</v>
       </c>
       <c r="AP2" s="9" t="s">
         <v>140</v>
@@ -1866,8 +1853,8 @@
       <c r="CB2" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="CC2" s="29" t="s">
-        <v>199</v>
+      <c r="CC2" s="28" t="s">
+        <v>194</v>
       </c>
       <c r="CD2" s="18" t="s">
         <v>146</v>
@@ -1994,13 +1981,13 @@
       <c r="A3" s="22"/>
       <c r="E3" s="3"/>
       <c r="F3" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>131</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>161</v>
@@ -2089,8 +2076,8 @@
       <c r="AN3" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="AO3" s="29" t="s">
-        <v>200</v>
+      <c r="AO3" s="28" t="s">
+        <v>195</v>
       </c>
       <c r="AP3" s="9" t="s">
         <v>140</v>
@@ -2194,8 +2181,8 @@
       <c r="CB3" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="CC3" s="29" t="s">
-        <v>200</v>
+      <c r="CC3" s="28" t="s">
+        <v>195</v>
       </c>
       <c r="CD3" s="18" t="s">
         <v>146</v>
@@ -4343,10 +4330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AM7"/>
+  <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4393,13 +4380,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -4511,10 +4498,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="27"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="F2" s="23" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>121</v>
@@ -4529,10 +4515,10 @@
         <v>156</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>165</v>
@@ -4556,29 +4542,28 @@
         <v>138</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U2" s="6"/>
+        <v>184</v>
+      </c>
       <c r="V2" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="W2" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Z2" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AC2" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AD2" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF2" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AG2" s="20">
         <v>45394</v>
@@ -4596,10 +4581,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="3" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="27"/>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="F3" s="23" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>121</v>
@@ -4614,10 +4598,10 @@
         <v>156</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M3" s="23" t="s">
         <v>165</v>
@@ -4641,29 +4625,28 @@
         <v>138</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U3" s="6"/>
+        <v>184</v>
+      </c>
       <c r="V3" s="23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="W3" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y3" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AC3" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AD3" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF3" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AG3" s="20">
         <v>45394</v>
@@ -4681,10 +4664,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="4" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="27"/>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="F4" s="23" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>121</v>
@@ -4702,7 +4684,7 @@
         <v>176</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>165</v>
@@ -4726,29 +4708,28 @@
         <v>138</v>
       </c>
       <c r="T4" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U4" s="6"/>
+        <v>184</v>
+      </c>
       <c r="V4" s="23" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="W4" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y4" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AC4" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AD4" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF4" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AG4" s="20">
         <v>45394</v>
@@ -4766,10 +4747,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="5" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="27"/>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="F5" s="23" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>121</v>
@@ -4784,10 +4764,10 @@
         <v>156</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="M5" s="23" t="s">
         <v>165</v>
@@ -4811,29 +4791,28 @@
         <v>138</v>
       </c>
       <c r="T5" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="V5" s="23" t="s">
         <v>188</v>
-      </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="23" t="s">
-        <v>192</v>
       </c>
       <c r="W5" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y5" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Z5" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AC5" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AD5" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF5" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AG5" s="20">
         <v>45394</v>
@@ -4851,10 +4830,9 @@
         <v>2958465</v>
       </c>
     </row>
-    <row r="6" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="27"/>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="F6" s="23" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>121</v>
@@ -4869,10 +4847,10 @@
         <v>156</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="M6" s="23" t="s">
         <v>165</v>
@@ -4896,29 +4874,28 @@
         <v>138</v>
       </c>
       <c r="T6" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U6" s="6"/>
+        <v>184</v>
+      </c>
       <c r="V6" s="23" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="W6" s="19" t="s">
         <v>158</v>
       </c>
       <c r="Y6" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Z6" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AC6" s="23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AD6" s="23" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF6" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AG6" s="20">
         <v>45394</v>
@@ -4933,91 +4910,6 @@
         <v>45394</v>
       </c>
       <c r="AM6" s="20">
-        <v>2958465</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="27"/>
-      <c r="F7" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="19">
-        <v>10</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="O7" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q7" s="23">
-        <v>33634</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="S7" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="T7" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="U7" s="6"/>
-      <c r="V7" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="W7" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y7" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC7" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="AD7" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="AF7" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="AG7" s="20">
-        <v>45394</v>
-      </c>
-      <c r="AH7" s="20">
-        <v>2958465</v>
-      </c>
-      <c r="AK7" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="AL7" s="20">
-        <v>45394</v>
-      </c>
-      <c r="AM7" s="20">
         <v>2958465</v>
       </c>
     </row>

</xml_diff>